<commit_message>
Media, Tests and Diagrams
</commit_message>
<xml_diff>
--- a/Project Schedule/Project_Schedule_220205.xlsx
+++ b/Project Schedule/Project_Schedule_220205.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Google Drive\Projects\BA\Project Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Google Drive\Projects\BA\reefing-system-docs\Project Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635C710C-39E2-4DD0-AEC4-AE541653DFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959AFD8A-5C9A-40E5-8DC8-36AA2DB33F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{67D3CC3D-E252-42CF-80D1-C55B726E9C49}"/>
   </bookViews>
@@ -165,19 +165,19 @@
     <t>Cutting Tests</t>
   </si>
   <si>
-    <t>Redundancy Tests</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
     <t>Actual</t>
   </si>
   <si>
-    <t>Submission date for thesis: 03.06.2022</t>
-  </si>
-  <si>
     <t>Submission date for abstract: xxxxxxx</t>
+  </si>
+  <si>
+    <t>Submission date for thesis: 04.06.2022</t>
+  </si>
+  <si>
+    <t>Additional Testing</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +239,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -617,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -650,7 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -665,10 +670,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -798,6 +807,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,7 +1135,7 @@
   <dimension ref="A1:AK76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="C43" sqref="C43:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,42 +1150,42 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="89"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="92"/>
+      <c r="AK1" s="92"/>
     </row>
     <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -1180,81 +1197,81 @@
       <c r="C2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="75">
+      <c r="D2" s="78">
         <v>6</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="68">
+      <c r="E2" s="72"/>
+      <c r="F2" s="71">
         <v>7</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="68">
+      <c r="G2" s="72"/>
+      <c r="H2" s="71">
         <v>8</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="68">
+      <c r="I2" s="72"/>
+      <c r="J2" s="71">
         <v>9</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="68">
+      <c r="K2" s="72"/>
+      <c r="L2" s="71">
         <v>10</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="68">
+      <c r="M2" s="72"/>
+      <c r="N2" s="71">
         <v>11</v>
       </c>
-      <c r="O2" s="74"/>
-      <c r="P2" s="69">
+      <c r="O2" s="77"/>
+      <c r="P2" s="72">
         <v>12</v>
       </c>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="68">
+      <c r="Q2" s="72"/>
+      <c r="R2" s="71">
         <v>13</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="68">
+      <c r="S2" s="72"/>
+      <c r="T2" s="71">
         <v>14</v>
       </c>
-      <c r="U2" s="69"/>
-      <c r="V2" s="68">
+      <c r="U2" s="72"/>
+      <c r="V2" s="71">
         <v>15</v>
       </c>
-      <c r="W2" s="69"/>
-      <c r="X2" s="68">
+      <c r="W2" s="72"/>
+      <c r="X2" s="71">
         <v>16</v>
       </c>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="68">
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="71">
         <v>17</v>
       </c>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="68">
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="71">
         <v>18</v>
       </c>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69">
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="72">
         <v>19</v>
       </c>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69">
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72">
         <v>20</v>
       </c>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="68">
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="71">
         <v>21</v>
       </c>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="68">
+      <c r="AI2" s="72"/>
+      <c r="AJ2" s="71">
         <v>22</v>
       </c>
-      <c r="AK2" s="88"/>
+      <c r="AK2" s="91"/>
     </row>
     <row r="3" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
       <c r="D3" s="24"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -1291,9 +1308,9 @@
       <c r="AK3" s="25"/>
     </row>
     <row r="4" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1330,14 +1347,16 @@
       <c r="AK4" s="4"/>
     </row>
     <row r="5" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="72">
+      <c r="B5" s="75">
         <v>12</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="41"/>
+      <c r="C5" s="75">
+        <v>8</v>
+      </c>
+      <c r="D5" s="40"/>
       <c r="E5" s="17"/>
       <c r="F5" s="21"/>
       <c r="G5" s="19"/>
@@ -1373,11 +1392,11 @@
       <c r="AK5" s="26"/>
     </row>
     <row r="6" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="19"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="21"/>
       <c r="G6" s="19"/>
       <c r="H6" s="21"/>
@@ -1412,14 +1431,16 @@
       <c r="AK6" s="26"/>
     </row>
     <row r="7" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="72">
+      <c r="B7" s="75">
         <v>12</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="75">
+        <v>8</v>
+      </c>
+      <c r="D7" s="28"/>
       <c r="E7" s="19"/>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
@@ -1455,12 +1476,12 @@
       <c r="AK7" s="26"/>
     </row>
     <row r="8" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="29"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="19"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="19"/>
       <c r="H8" s="21"/>
       <c r="I8" s="19"/>
@@ -1494,14 +1515,16 @@
       <c r="AK8" s="26"/>
     </row>
     <row r="9" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="72">
+      <c r="B9" s="75">
         <v>5</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="75">
+        <v>10</v>
+      </c>
+      <c r="D9" s="28"/>
       <c r="E9" s="19"/>
       <c r="F9" s="21"/>
       <c r="G9" s="17"/>
@@ -1537,14 +1560,14 @@
       <c r="AK9" s="26"/>
     </row>
     <row r="10" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
       <c r="I10" s="19"/>
       <c r="J10" s="21"/>
       <c r="K10" s="19"/>
@@ -1576,93 +1599,95 @@
       <c r="AK10" s="26"/>
     </row>
     <row r="11" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="31"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="31"/>
-      <c r="Z11" s="31"/>
-      <c r="AA11" s="31"/>
-      <c r="AB11" s="31"/>
-      <c r="AC11" s="31"/>
-      <c r="AD11" s="34"/>
-      <c r="AE11" s="34"/>
-      <c r="AF11" s="31"/>
-      <c r="AG11" s="31"/>
-      <c r="AH11" s="31"/>
-      <c r="AI11" s="31"/>
-      <c r="AJ11" s="31"/>
-      <c r="AK11" s="35"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="30"/>
+      <c r="AK11" s="34"/>
     </row>
     <row r="12" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="33"/>
-      <c r="U12" s="33"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
-      <c r="X12" s="33"/>
-      <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="33"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="33"/>
-      <c r="AD12" s="34"/>
-      <c r="AE12" s="34"/>
-      <c r="AF12" s="33"/>
-      <c r="AG12" s="33"/>
-      <c r="AH12" s="33"/>
-      <c r="AI12" s="33"/>
-      <c r="AJ12" s="33"/>
-      <c r="AK12" s="36"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="33"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
+      <c r="AI12" s="32"/>
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="35"/>
     </row>
     <row r="13" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="72">
+      <c r="B13" s="75">
         <v>12</v>
       </c>
-      <c r="C13" s="72"/>
+      <c r="C13" s="75">
+        <v>12</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="21"/>
@@ -1699,13 +1724,13 @@
       <c r="AK13" s="26"/>
     </row>
     <row r="14" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="21"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
@@ -1738,13 +1763,15 @@
       <c r="AK14" s="26"/>
     </row>
     <row r="15" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="72">
+      <c r="B15" s="75">
         <v>12</v>
       </c>
-      <c r="C15" s="72"/>
+      <c r="C15" s="75">
+        <v>10</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="21"/>
@@ -1781,15 +1808,15 @@
       <c r="AK15" s="26"/>
     </row>
     <row r="16" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="A16" s="74"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="19"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="21"/>
       <c r="K16" s="19"/>
       <c r="L16" s="21"/>
@@ -1820,13 +1847,15 @@
       <c r="AK16" s="26"/>
     </row>
     <row r="17" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="72">
+      <c r="B17" s="75">
         <v>8</v>
       </c>
-      <c r="C17" s="72"/>
+      <c r="C17" s="75">
+        <v>6</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
       <c r="F17" s="21"/>
@@ -1863,9 +1892,9 @@
       <c r="AK17" s="26"/>
     </row>
     <row r="18" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="21"/>
@@ -1873,8 +1902,8 @@
       <c r="H18" s="21"/>
       <c r="I18" s="19"/>
       <c r="J18" s="21"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="21"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
       <c r="M18" s="19"/>
       <c r="N18" s="21"/>
       <c r="O18" s="19"/>
@@ -1902,94 +1931,96 @@
       <c r="AK18" s="26"/>
     </row>
     <row r="19" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="31"/>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="31"/>
-      <c r="AB19" s="31"/>
-      <c r="AC19" s="31"/>
-      <c r="AD19" s="34"/>
-      <c r="AE19" s="34"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="31"/>
-      <c r="AJ19" s="31"/>
-      <c r="AK19" s="35"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="30"/>
+      <c r="AA19" s="30"/>
+      <c r="AB19" s="30"/>
+      <c r="AC19" s="30"/>
+      <c r="AD19" s="33"/>
+      <c r="AE19" s="33"/>
+      <c r="AF19" s="30"/>
+      <c r="AG19" s="30"/>
+      <c r="AH19" s="30"/>
+      <c r="AI19" s="30"/>
+      <c r="AJ19" s="30"/>
+      <c r="AK19" s="34"/>
     </row>
     <row r="20" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="33"/>
-      <c r="AD20" s="34"/>
-      <c r="AE20" s="34"/>
-      <c r="AF20" s="33"/>
-      <c r="AG20" s="33"/>
-      <c r="AH20" s="33"/>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="33"/>
-      <c r="AK20" s="36"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="32"/>
+      <c r="AB20" s="32"/>
+      <c r="AC20" s="32"/>
+      <c r="AD20" s="33"/>
+      <c r="AE20" s="33"/>
+      <c r="AF20" s="32"/>
+      <c r="AG20" s="32"/>
+      <c r="AH20" s="32"/>
+      <c r="AI20" s="32"/>
+      <c r="AJ20" s="32"/>
+      <c r="AK20" s="35"/>
     </row>
     <row r="21" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="72">
+      <c r="B21" s="75">
         <v>5</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="75">
+        <v>2</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="19"/>
       <c r="F21" s="21"/>
       <c r="G21" s="19"/>
@@ -2011,30 +2042,30 @@
       <c r="W21" s="19"/>
       <c r="X21" s="21"/>
       <c r="Y21" s="19"/>
-      <c r="Z21" s="44"/>
-      <c r="AA21" s="33"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="32"/>
       <c r="AB21" s="21"/>
       <c r="AC21" s="19"/>
       <c r="AD21" s="21"/>
       <c r="AE21" s="19"/>
       <c r="AF21" s="21"/>
-      <c r="AG21" s="33"/>
-      <c r="AH21" s="44"/>
-      <c r="AI21" s="33"/>
+      <c r="AG21" s="32"/>
+      <c r="AH21" s="42"/>
+      <c r="AI21" s="32"/>
       <c r="AJ21" s="21"/>
       <c r="AK21" s="26"/>
     </row>
     <row r="22" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="29"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="19"/>
       <c r="F22" s="21"/>
       <c r="G22" s="19"/>
       <c r="H22" s="21"/>
       <c r="I22" s="19"/>
-      <c r="J22" s="21"/>
+      <c r="J22" s="46"/>
       <c r="K22" s="22"/>
       <c r="L22" s="21"/>
       <c r="M22" s="19"/>
@@ -2064,14 +2095,16 @@
       <c r="AK22" s="26"/>
     </row>
     <row r="23" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="72">
+      <c r="B23" s="75">
         <v>20</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="75">
+        <v>24</v>
+      </c>
+      <c r="D23" s="28"/>
       <c r="E23" s="19"/>
       <c r="F23" s="21"/>
       <c r="G23" s="19"/>
@@ -2107,9 +2140,9 @@
       <c r="AK23" s="26"/>
     </row>
     <row r="24" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
@@ -2117,8 +2150,8 @@
       <c r="H24" s="11"/>
       <c r="I24" s="10"/>
       <c r="J24" s="21"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="21"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="46"/>
       <c r="M24" s="19"/>
       <c r="N24" s="21"/>
       <c r="O24" s="22"/>
@@ -2146,14 +2179,16 @@
       <c r="AK24" s="26"/>
     </row>
     <row r="25" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="72">
+      <c r="B25" s="75">
         <v>24</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="29"/>
+      <c r="C25" s="75">
+        <v>20</v>
+      </c>
+      <c r="D25" s="28"/>
       <c r="E25" s="19"/>
       <c r="F25" s="21"/>
       <c r="G25" s="19"/>
@@ -2189,9 +2224,9 @@
       <c r="AK25" s="26"/>
     </row>
     <row r="26" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="21"/>
@@ -2200,8 +2235,8 @@
       <c r="I26" s="19"/>
       <c r="J26" s="21"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="19"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="45"/>
       <c r="N26" s="21"/>
       <c r="O26" s="12"/>
       <c r="P26" s="19"/>
@@ -2228,13 +2263,15 @@
       <c r="AK26" s="26"/>
     </row>
     <row r="27" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="70" t="s">
+      <c r="A27" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="72">
+      <c r="B27" s="75">
         <v>20</v>
       </c>
-      <c r="C27" s="72"/>
+      <c r="C27" s="75">
+        <v>18</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
       <c r="F27" s="21"/>
@@ -2243,10 +2280,10 @@
       <c r="I27" s="19"/>
       <c r="J27" s="21"/>
       <c r="K27" s="19"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="33"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="32"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="21"/>
@@ -2271,9 +2308,9 @@
       <c r="AK27" s="26"/>
     </row>
     <row r="28" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="21"/>
@@ -2284,7 +2321,7 @@
       <c r="K28" s="19"/>
       <c r="L28" s="21"/>
       <c r="M28" s="19"/>
-      <c r="N28" s="21"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="19"/>
       <c r="P28" s="21"/>
       <c r="Q28" s="19"/>
@@ -2310,13 +2347,15 @@
       <c r="AK28" s="26"/>
     </row>
     <row r="29" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="72">
+      <c r="B29" s="75">
         <v>36</v>
       </c>
-      <c r="C29" s="72"/>
+      <c r="C29" s="75">
+        <v>30</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="21"/>
@@ -2353,9 +2392,9 @@
       <c r="AK29" s="26"/>
     </row>
     <row r="30" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="21"/>
@@ -2371,15 +2410,15 @@
       <c r="P30" s="21"/>
       <c r="Q30" s="19"/>
       <c r="R30" s="21"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="19"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="45"/>
       <c r="V30" s="21"/>
       <c r="W30" s="19"/>
       <c r="X30" s="21"/>
       <c r="Y30" s="19"/>
       <c r="Z30" s="21"/>
-      <c r="AA30" s="19"/>
+      <c r="AA30" s="45"/>
       <c r="AB30" s="21"/>
       <c r="AC30" s="19"/>
       <c r="AD30" s="21"/>
@@ -2392,13 +2431,15 @@
       <c r="AK30" s="26"/>
     </row>
     <row r="31" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="72">
+      <c r="B31" s="75">
         <v>12</v>
       </c>
-      <c r="C31" s="72"/>
+      <c r="C31" s="75">
+        <v>18</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
       <c r="F31" s="21"/>
@@ -2407,8 +2448,8 @@
       <c r="I31" s="19"/>
       <c r="J31" s="21"/>
       <c r="K31" s="19"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="33"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="21"/>
       <c r="O31" s="19"/>
       <c r="P31" s="21"/>
@@ -2435,169 +2476,171 @@
       <c r="AK31" s="26"/>
     </row>
     <row r="32" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
+      <c r="A32" s="74"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="31"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="30"/>
       <c r="V32" s="11"/>
       <c r="W32" s="10"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="31"/>
-      <c r="Z32" s="21"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="46"/>
       <c r="AA32" s="19"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="19"/>
       <c r="AD32" s="21"/>
-      <c r="AE32" s="19"/>
+      <c r="AE32" s="45"/>
       <c r="AF32" s="21"/>
       <c r="AG32" s="19"/>
       <c r="AH32" s="21"/>
       <c r="AI32" s="19"/>
-      <c r="AJ32" s="42"/>
-      <c r="AK32" s="35"/>
+      <c r="AJ32" s="41"/>
+      <c r="AK32" s="34"/>
     </row>
     <row r="33" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="84" t="s">
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="85"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-      <c r="U33" s="31"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="31"/>
-      <c r="Z33" s="31"/>
-      <c r="AA33" s="31"/>
-      <c r="AB33" s="31"/>
-      <c r="AC33" s="31"/>
-      <c r="AD33" s="31"/>
-      <c r="AE33" s="31"/>
-      <c r="AF33" s="31"/>
-      <c r="AG33" s="31"/>
-      <c r="AH33" s="31"/>
-      <c r="AI33" s="31"/>
-      <c r="AJ33" s="31"/>
-      <c r="AK33" s="35"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="30"/>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="30"/>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="30"/>
+      <c r="AG33" s="30"/>
+      <c r="AH33" s="30"/>
+      <c r="AI33" s="30"/>
+      <c r="AJ33" s="30"/>
+      <c r="AK33" s="34"/>
     </row>
     <row r="34" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="86"/>
-      <c r="Q34" s="87"/>
-      <c r="R34" s="33"/>
-      <c r="S34" s="33"/>
-      <c r="T34" s="33"/>
-      <c r="U34" s="33"/>
-      <c r="X34" s="33"/>
-      <c r="Y34" s="33"/>
-      <c r="Z34" s="33"/>
-      <c r="AA34" s="33"/>
-      <c r="AB34" s="33"/>
-      <c r="AC34" s="33"/>
-      <c r="AD34" s="33"/>
-      <c r="AE34" s="33"/>
-      <c r="AF34" s="33"/>
-      <c r="AG34" s="33"/>
-      <c r="AH34" s="33"/>
-      <c r="AI34" s="33"/>
-      <c r="AJ34" s="33"/>
-      <c r="AK34" s="36"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="32"/>
+      <c r="AB34" s="32"/>
+      <c r="AC34" s="32"/>
+      <c r="AD34" s="32"/>
+      <c r="AE34" s="32"/>
+      <c r="AF34" s="32"/>
+      <c r="AG34" s="32"/>
+      <c r="AH34" s="32"/>
+      <c r="AI34" s="32"/>
+      <c r="AJ34" s="32"/>
+      <c r="AK34" s="35"/>
     </row>
     <row r="35" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="72">
+      <c r="B35" s="75">
         <v>8</v>
       </c>
-      <c r="C35" s="72"/>
+      <c r="C35" s="75">
+        <v>10</v>
+      </c>
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="33"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="33"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="42"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="32"/>
       <c r="V35" s="21"/>
       <c r="W35" s="19"/>
-      <c r="X35" s="44"/>
-      <c r="Y35" s="33"/>
-      <c r="Z35" s="44"/>
-      <c r="AA35" s="33"/>
-      <c r="AB35" s="44"/>
-      <c r="AC35" s="33"/>
-      <c r="AD35" s="44"/>
-      <c r="AE35" s="33"/>
-      <c r="AF35" s="44"/>
-      <c r="AG35" s="33"/>
-      <c r="AH35" s="44"/>
-      <c r="AI35" s="33"/>
-      <c r="AJ35" s="44"/>
-      <c r="AK35" s="36"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="42"/>
+      <c r="AA35" s="32"/>
+      <c r="AB35" s="42"/>
+      <c r="AC35" s="32"/>
+      <c r="AD35" s="42"/>
+      <c r="AE35" s="32"/>
+      <c r="AF35" s="42"/>
+      <c r="AG35" s="32"/>
+      <c r="AH35" s="42"/>
+      <c r="AI35" s="32"/>
+      <c r="AJ35" s="42"/>
+      <c r="AK35" s="35"/>
     </row>
     <row r="36" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
       <c r="F36" s="21"/>
@@ -2611,10 +2654,10 @@
       <c r="N36" s="21"/>
       <c r="O36" s="22"/>
       <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
+      <c r="Q36" s="45"/>
       <c r="R36" s="21"/>
       <c r="S36" s="19"/>
-      <c r="T36" s="42"/>
+      <c r="T36" s="41"/>
       <c r="U36" s="19"/>
       <c r="V36" s="21"/>
       <c r="W36" s="19"/>
@@ -2634,13 +2677,15 @@
       <c r="AK36" s="26"/>
     </row>
     <row r="37" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="72">
+      <c r="B37" s="75">
         <v>5</v>
       </c>
-      <c r="C37" s="72"/>
+      <c r="C37" s="75">
+        <v>8</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
       <c r="F37" s="21"/>
@@ -2677,9 +2722,9 @@
       <c r="AK37" s="26"/>
     </row>
     <row r="38" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="21"/>
@@ -2693,8 +2738,8 @@
       <c r="N38" s="21"/>
       <c r="O38" s="22"/>
       <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="21"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="46"/>
       <c r="S38" s="19"/>
       <c r="T38" s="21"/>
       <c r="U38" s="19"/>
@@ -2716,13 +2761,15 @@
       <c r="AK38" s="26"/>
     </row>
     <row r="39" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="70" t="s">
+      <c r="A39" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="72">
+      <c r="B39" s="75">
         <v>8</v>
       </c>
-      <c r="C39" s="72"/>
+      <c r="C39" s="75">
+        <v>4</v>
+      </c>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="21"/>
@@ -2759,9 +2806,9 @@
       <c r="AK39" s="26"/>
     </row>
     <row r="40" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="71"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="73"/>
+      <c r="A40" s="74"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="21"/>
@@ -2780,7 +2827,7 @@
       <c r="S40" s="19"/>
       <c r="T40" s="21"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="21"/>
+      <c r="V40" s="46"/>
       <c r="W40" s="19"/>
       <c r="X40" s="21"/>
       <c r="Y40" s="19"/>
@@ -2798,13 +2845,15 @@
       <c r="AK40" s="26"/>
     </row>
     <row r="41" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="72">
+      <c r="B41" s="75">
         <v>20</v>
       </c>
-      <c r="C41" s="72"/>
+      <c r="C41" s="75">
+        <v>18</v>
+      </c>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
       <c r="F41" s="21"/>
@@ -2841,9 +2890,9 @@
       <c r="AK41" s="26"/>
     </row>
     <row r="42" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="21"/>
@@ -2863,8 +2912,8 @@
       <c r="T42" s="21"/>
       <c r="U42" s="19"/>
       <c r="V42" s="21"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="21"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="46"/>
       <c r="Y42" s="19"/>
       <c r="Z42" s="21"/>
       <c r="AA42" s="19"/>
@@ -2880,13 +2929,15 @@
       <c r="AK42" s="26"/>
     </row>
     <row r="43" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="70" t="s">
+      <c r="A43" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="72">
+      <c r="B43" s="75">
         <v>15</v>
       </c>
-      <c r="C43" s="72"/>
+      <c r="C43" s="75">
+        <v>24</v>
+      </c>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
       <c r="F43" s="21"/>
@@ -2923,9 +2974,9 @@
       <c r="AK43" s="26"/>
     </row>
     <row r="44" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
       <c r="F44" s="21"/>
@@ -2946,8 +2997,8 @@
       <c r="U44" s="19"/>
       <c r="V44" s="21"/>
       <c r="W44" s="19"/>
-      <c r="X44" s="21"/>
-      <c r="Y44" s="19"/>
+      <c r="X44" s="46"/>
+      <c r="Y44" s="45"/>
       <c r="Z44" s="21"/>
       <c r="AA44" s="19"/>
       <c r="AB44" s="21"/>
@@ -2962,13 +3013,15 @@
       <c r="AK44" s="26"/>
     </row>
     <row r="45" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="70" t="s">
+      <c r="A45" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="72">
+      <c r="B45" s="75">
         <v>20</v>
       </c>
-      <c r="C45" s="72"/>
+      <c r="C45" s="75">
+        <v>36</v>
+      </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
       <c r="F45" s="21"/>
@@ -3005,9 +3058,9 @@
       <c r="AK45" s="26"/>
     </row>
     <row r="46" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
+      <c r="A46" s="74"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
       <c r="F46" s="21"/>
@@ -3029,9 +3082,9 @@
       <c r="V46" s="21"/>
       <c r="W46" s="19"/>
       <c r="X46" s="21"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
+      <c r="Y46" s="45"/>
+      <c r="Z46" s="45"/>
+      <c r="AA46" s="45"/>
       <c r="AB46" s="21"/>
       <c r="AC46" s="19"/>
       <c r="AD46" s="21"/>
@@ -3044,91 +3097,93 @@
       <c r="AK46" s="26"/>
     </row>
     <row r="47" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="82" t="s">
+      <c r="A47" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
+      <c r="B47" s="79"/>
+      <c r="C47" s="79"/>
       <c r="D47" s="5"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="31"/>
-      <c r="S47" s="31"/>
-      <c r="T47" s="31"/>
-      <c r="U47" s="31"/>
-      <c r="V47" s="31"/>
-      <c r="W47" s="31"/>
-      <c r="Z47" s="31"/>
-      <c r="AA47" s="31"/>
-      <c r="AB47" s="31"/>
-      <c r="AC47" s="31"/>
-      <c r="AD47" s="84" t="s">
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="30"/>
+      <c r="W47" s="30"/>
+      <c r="Z47" s="30"/>
+      <c r="AA47" s="30"/>
+      <c r="AB47" s="30"/>
+      <c r="AC47" s="30"/>
+      <c r="AD47" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AE47" s="85"/>
-      <c r="AF47" s="31"/>
-      <c r="AG47" s="31"/>
-      <c r="AH47" s="31"/>
-      <c r="AI47" s="31"/>
-      <c r="AJ47" s="31"/>
-      <c r="AK47" s="35"/>
+      <c r="AE47" s="88"/>
+      <c r="AF47" s="30"/>
+      <c r="AG47" s="30"/>
+      <c r="AH47" s="30"/>
+      <c r="AI47" s="30"/>
+      <c r="AJ47" s="30"/>
+      <c r="AK47" s="34"/>
     </row>
     <row r="48" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="81"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="77"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
       <c r="D48" s="2"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
-      <c r="N48" s="33"/>
-      <c r="O48" s="33"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
-      <c r="R48" s="33"/>
-      <c r="S48" s="33"/>
-      <c r="T48" s="33"/>
-      <c r="U48" s="33"/>
-      <c r="V48" s="33"/>
-      <c r="W48" s="33"/>
-      <c r="Z48" s="33"/>
-      <c r="AA48" s="33"/>
-      <c r="AB48" s="33"/>
-      <c r="AC48" s="33"/>
-      <c r="AD48" s="86"/>
-      <c r="AE48" s="87"/>
-      <c r="AF48" s="33"/>
-      <c r="AG48" s="33"/>
-      <c r="AH48" s="33"/>
-      <c r="AI48" s="33"/>
-      <c r="AJ48" s="33"/>
-      <c r="AK48" s="36"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="32"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="32"/>
+      <c r="W48" s="32"/>
+      <c r="Z48" s="32"/>
+      <c r="AA48" s="32"/>
+      <c r="AB48" s="32"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="89"/>
+      <c r="AE48" s="90"/>
+      <c r="AF48" s="32"/>
+      <c r="AG48" s="32"/>
+      <c r="AH48" s="32"/>
+      <c r="AI48" s="32"/>
+      <c r="AJ48" s="32"/>
+      <c r="AK48" s="35"/>
     </row>
     <row r="49" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="70" t="s">
+      <c r="A49" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="72">
+      <c r="B49" s="75">
         <v>8</v>
       </c>
-      <c r="C49" s="72"/>
+      <c r="C49" s="75">
+        <v>10</v>
+      </c>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
       <c r="F49" s="21"/>
@@ -3165,9 +3220,9 @@
       <c r="AK49" s="26"/>
     </row>
     <row r="50" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="71"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="73"/>
+      <c r="A50" s="74"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="76"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="21"/>
@@ -3192,7 +3247,7 @@
       <c r="Y50" s="19"/>
       <c r="Z50" s="21"/>
       <c r="AA50" s="19"/>
-      <c r="AB50" s="21"/>
+      <c r="AB50" s="46"/>
       <c r="AC50" s="19"/>
       <c r="AD50" s="21"/>
       <c r="AE50" s="19"/>
@@ -3204,13 +3259,15 @@
       <c r="AK50" s="26"/>
     </row>
     <row r="51" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="70" t="s">
+      <c r="A51" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="72">
+      <c r="B51" s="75">
         <v>5</v>
       </c>
-      <c r="C51" s="72"/>
+      <c r="C51" s="75">
+        <v>8</v>
+      </c>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
       <c r="F51" s="21"/>
@@ -3247,9 +3304,9 @@
       <c r="AK51" s="26"/>
     </row>
     <row r="52" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
-      <c r="B52" s="73"/>
-      <c r="C52" s="73"/>
+      <c r="A52" s="74"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="76"/>
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
       <c r="F52" s="21"/>
@@ -3274,9 +3331,9 @@
       <c r="Y52" s="19"/>
       <c r="Z52" s="21"/>
       <c r="AA52" s="19"/>
-      <c r="AB52" s="21"/>
-      <c r="AC52" s="19"/>
-      <c r="AD52" s="21"/>
+      <c r="AB52" s="46"/>
+      <c r="AC52" s="45"/>
+      <c r="AD52" s="46"/>
       <c r="AE52" s="19"/>
       <c r="AF52" s="21"/>
       <c r="AG52" s="19"/>
@@ -3286,13 +3343,15 @@
       <c r="AK52" s="26"/>
     </row>
     <row r="53" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="72">
+      <c r="A53" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="75">
         <v>5</v>
       </c>
-      <c r="C53" s="72"/>
+      <c r="C53" s="75">
+        <v>12</v>
+      </c>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
       <c r="F53" s="21"/>
@@ -3329,9 +3388,9 @@
       <c r="AK53" s="26"/>
     </row>
     <row r="54" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="71"/>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
+      <c r="A54" s="74"/>
+      <c r="B54" s="76"/>
+      <c r="C54" s="76"/>
       <c r="D54" s="9"/>
       <c r="E54" s="10"/>
       <c r="F54" s="21"/>
@@ -3358,102 +3417,104 @@
       <c r="AA54" s="19"/>
       <c r="AB54" s="21"/>
       <c r="AC54" s="19"/>
-      <c r="AD54" s="21"/>
-      <c r="AE54" s="19"/>
-      <c r="AF54" s="21"/>
-      <c r="AG54" s="19"/>
-      <c r="AH54" s="21"/>
+      <c r="AD54" s="46"/>
+      <c r="AE54" s="45"/>
+      <c r="AF54" s="46"/>
+      <c r="AG54" s="45"/>
+      <c r="AH54" s="46"/>
       <c r="AI54" s="19"/>
       <c r="AJ54" s="21"/>
       <c r="AK54" s="26"/>
     </row>
     <row r="55" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="82" t="s">
+      <c r="A55" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="76"/>
-      <c r="C55" s="76"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="79"/>
       <c r="D55" s="5"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31"/>
-      <c r="M55" s="31"/>
-      <c r="N55" s="31"/>
-      <c r="O55" s="31"/>
-      <c r="P55" s="31"/>
-      <c r="Q55" s="31"/>
-      <c r="R55" s="31"/>
-      <c r="S55" s="31"/>
-      <c r="T55" s="31"/>
-      <c r="U55" s="31"/>
-      <c r="V55" s="31"/>
-      <c r="W55" s="31"/>
-      <c r="X55" s="31"/>
-      <c r="Y55" s="31"/>
-      <c r="Z55" s="31"/>
-      <c r="AC55" s="31"/>
-      <c r="AD55" s="34"/>
-      <c r="AE55" s="34"/>
-      <c r="AF55" s="31"/>
-      <c r="AG55" s="84" t="s">
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="30"/>
+      <c r="L55" s="30"/>
+      <c r="M55" s="30"/>
+      <c r="N55" s="30"/>
+      <c r="O55" s="30"/>
+      <c r="P55" s="30"/>
+      <c r="Q55" s="30"/>
+      <c r="R55" s="30"/>
+      <c r="S55" s="30"/>
+      <c r="T55" s="30"/>
+      <c r="U55" s="30"/>
+      <c r="V55" s="30"/>
+      <c r="W55" s="30"/>
+      <c r="X55" s="30"/>
+      <c r="Y55" s="30"/>
+      <c r="Z55" s="30"/>
+      <c r="AC55" s="30"/>
+      <c r="AD55" s="33"/>
+      <c r="AE55" s="33"/>
+      <c r="AF55" s="30"/>
+      <c r="AG55" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="85"/>
-      <c r="AI55" s="31"/>
-      <c r="AJ55" s="31"/>
-      <c r="AK55" s="35"/>
+      <c r="AH55" s="88"/>
+      <c r="AI55" s="30"/>
+      <c r="AJ55" s="30"/>
+      <c r="AK55" s="34"/>
     </row>
     <row r="56" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="81"/>
-      <c r="B56" s="77"/>
-      <c r="C56" s="77"/>
+      <c r="A56" s="84"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="80"/>
       <c r="D56" s="2"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
-      <c r="O56" s="33"/>
-      <c r="P56" s="33"/>
-      <c r="Q56" s="33"/>
-      <c r="R56" s="33"/>
-      <c r="S56" s="33"/>
-      <c r="T56" s="33"/>
-      <c r="U56" s="33"/>
-      <c r="V56" s="33"/>
-      <c r="W56" s="33"/>
-      <c r="X56" s="33"/>
-      <c r="Y56" s="33"/>
-      <c r="Z56" s="33"/>
-      <c r="AC56" s="33"/>
-      <c r="AD56" s="34"/>
-      <c r="AE56" s="34"/>
-      <c r="AF56" s="33"/>
-      <c r="AG56" s="86"/>
-      <c r="AH56" s="87"/>
-      <c r="AI56" s="33"/>
-      <c r="AJ56" s="33"/>
-      <c r="AK56" s="36"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="32"/>
+      <c r="N56" s="32"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="32"/>
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="32"/>
+      <c r="V56" s="32"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="32"/>
+      <c r="Y56" s="32"/>
+      <c r="Z56" s="32"/>
+      <c r="AC56" s="32"/>
+      <c r="AD56" s="33"/>
+      <c r="AE56" s="33"/>
+      <c r="AF56" s="32"/>
+      <c r="AG56" s="89"/>
+      <c r="AH56" s="90"/>
+      <c r="AI56" s="32"/>
+      <c r="AJ56" s="32"/>
+      <c r="AK56" s="35"/>
     </row>
     <row r="57" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="53" t="s">
+      <c r="A57" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="63">
+      <c r="B57" s="66">
         <v>76</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="41"/>
+      <c r="C57" s="66">
+        <v>100</v>
+      </c>
+      <c r="D57" s="40"/>
       <c r="E57" s="17"/>
       <c r="F57" s="16"/>
       <c r="G57" s="22"/>
@@ -3489,12 +3550,12 @@
       <c r="AK57" s="27"/>
     </row>
     <row r="58" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="71"/>
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
+      <c r="A58" s="74"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="76"/>
       <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="21"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="46"/>
       <c r="G58" s="19"/>
       <c r="H58" s="21"/>
       <c r="I58" s="19"/>
@@ -3506,35 +3567,37 @@
       <c r="O58" s="22"/>
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>
-      <c r="R58" s="21"/>
+      <c r="R58" s="46"/>
       <c r="S58" s="19"/>
       <c r="T58" s="21"/>
       <c r="U58" s="19"/>
       <c r="V58" s="21"/>
-      <c r="W58" s="19"/>
-      <c r="X58" s="21"/>
+      <c r="W58" s="45"/>
+      <c r="X58" s="46"/>
       <c r="Y58" s="19"/>
       <c r="Z58" s="21"/>
       <c r="AA58" s="19"/>
       <c r="AB58" s="21"/>
       <c r="AC58" s="19"/>
-      <c r="AD58" s="34"/>
-      <c r="AE58" s="34"/>
-      <c r="AF58" s="19"/>
-      <c r="AG58" s="19"/>
-      <c r="AH58" s="21"/>
-      <c r="AI58" s="19"/>
-      <c r="AJ58" s="21"/>
-      <c r="AK58" s="26"/>
+      <c r="AD58" s="33"/>
+      <c r="AE58" s="95"/>
+      <c r="AF58" s="45"/>
+      <c r="AG58" s="45"/>
+      <c r="AH58" s="46"/>
+      <c r="AI58" s="45"/>
+      <c r="AJ58" s="46"/>
+      <c r="AK58" s="96"/>
     </row>
     <row r="59" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="63">
+      <c r="B59" s="66">
         <v>12</v>
       </c>
-      <c r="C59" s="63"/>
+      <c r="C59" s="66">
+        <v>8</v>
+      </c>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
       <c r="F59" s="21"/>
@@ -3564,316 +3627,315 @@
       <c r="AD59" s="21"/>
       <c r="AE59" s="19"/>
       <c r="AF59" s="21"/>
-      <c r="AG59" s="17"/>
+      <c r="AG59" s="100"/>
       <c r="AH59" s="21"/>
-      <c r="AI59" s="19"/>
+      <c r="AI59" s="17"/>
       <c r="AJ59" s="16"/>
       <c r="AK59" s="27"/>
     </row>
     <row r="60" spans="1:37" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="48"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
+      <c r="A60" s="51"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
       <c r="D60" s="13"/>
       <c r="E60" s="14"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="39"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="37"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="37"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="36"/>
       <c r="S60" s="14"/>
       <c r="T60" s="15"/>
       <c r="U60" s="14"/>
       <c r="V60" s="15"/>
-      <c r="W60" s="38"/>
-      <c r="X60" s="37"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="37"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="37"/>
-      <c r="AC60" s="38"/>
-      <c r="AD60" s="37"/>
-      <c r="AE60" s="38"/>
-      <c r="AF60" s="37"/>
-      <c r="AG60" s="38"/>
-      <c r="AH60" s="37"/>
-      <c r="AI60" s="38"/>
-      <c r="AJ60" s="15"/>
-      <c r="AK60" s="28"/>
+      <c r="W60" s="37"/>
+      <c r="X60" s="36"/>
+      <c r="Y60" s="37"/>
+      <c r="Z60" s="36"/>
+      <c r="AA60" s="37"/>
+      <c r="AB60" s="36"/>
+      <c r="AC60" s="37"/>
+      <c r="AD60" s="36"/>
+      <c r="AE60" s="37"/>
+      <c r="AF60" s="98"/>
+      <c r="AG60" s="99"/>
+      <c r="AH60" s="93"/>
+      <c r="AI60" s="94"/>
+      <c r="AJ60" s="93"/>
+      <c r="AK60" s="97"/>
     </row>
     <row r="61" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="58">
+      <c r="B61" s="61">
         <f>SUM(B5:B60)</f>
         <v>360</v>
       </c>
-      <c r="C61" s="58"/>
-      <c r="W61" s="40"/>
-      <c r="X61" s="40"/>
-      <c r="Y61" s="40"/>
-      <c r="AB61" s="40"/>
-      <c r="AC61" s="40"/>
-      <c r="AF61" s="78" t="s">
+      <c r="C61" s="61">
+        <f>SUM(C5:C60)</f>
+        <v>404</v>
+      </c>
+      <c r="W61" s="39"/>
+      <c r="X61" s="39"/>
+      <c r="Y61" s="39"/>
+      <c r="AB61" s="39"/>
+      <c r="AC61" s="39"/>
+      <c r="AH61" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="AG61" s="79"/>
-      <c r="AH61" s="40"/>
-      <c r="AI61" s="40"/>
-      <c r="AJ61" s="78" t="s">
+      <c r="AI61" s="82"/>
+      <c r="AJ61" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="AK61" s="79"/>
+      <c r="AK61" s="82"/>
     </row>
     <row r="62" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="W62" s="40"/>
-      <c r="X62" s="40"/>
-      <c r="Y62" s="40"/>
-      <c r="AB62" s="40"/>
-      <c r="AC62" s="40"/>
-      <c r="AF62" s="78"/>
-      <c r="AG62" s="79"/>
-      <c r="AH62" s="40"/>
-      <c r="AI62" s="40"/>
-      <c r="AJ62" s="78"/>
-      <c r="AK62" s="79"/>
+      <c r="A62" s="68"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
+      <c r="W62" s="39"/>
+      <c r="X62" s="39"/>
+      <c r="Y62" s="39"/>
+      <c r="AB62" s="39"/>
+      <c r="AC62" s="39"/>
+      <c r="AH62" s="81"/>
+      <c r="AI62" s="82"/>
+      <c r="AJ62" s="81"/>
+      <c r="AK62" s="82"/>
     </row>
     <row r="63" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="W63" s="40"/>
-      <c r="X63" s="40"/>
-      <c r="Y63" s="40"/>
-      <c r="Z63" s="40"/>
-      <c r="AA63" s="40"/>
-      <c r="AB63" s="40"/>
-      <c r="AC63" s="40"/>
-      <c r="AD63" s="40"/>
-      <c r="AE63" s="40"/>
-      <c r="AF63" s="40"/>
-      <c r="AG63" s="40"/>
-      <c r="AH63" s="40"/>
-      <c r="AI63" s="40"/>
+      <c r="A63" s="60"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="61"/>
+      <c r="W63" s="39"/>
+      <c r="X63" s="39"/>
+      <c r="Y63" s="39"/>
+      <c r="Z63" s="39"/>
+      <c r="AA63" s="39"/>
+      <c r="AB63" s="39"/>
+      <c r="AC63" s="39"/>
+      <c r="AD63" s="39"/>
+      <c r="AE63" s="39"/>
+      <c r="AF63" s="39"/>
+      <c r="AG63" s="39"/>
+      <c r="AH63" s="39"/>
+      <c r="AI63" s="39"/>
     </row>
     <row r="64" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="57"/>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
+      <c r="A64" s="60"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
     </row>
     <row r="65" spans="4:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="66" t="s">
+      <c r="D65" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="70"/>
+      <c r="F65" s="70"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="70"/>
+      <c r="J65" s="70"/>
+      <c r="K65" s="70"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="63"/>
+      <c r="O65" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="P65" s="54"/>
+      <c r="Q65" s="54"/>
+      <c r="R65" s="54"/>
+      <c r="S65" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="T65" s="54"/>
+      <c r="U65" s="54"/>
+      <c r="V65" s="54"/>
+      <c r="W65" s="54"/>
+      <c r="X65" s="54"/>
+      <c r="Y65" s="54"/>
+      <c r="Z65" s="54"/>
+      <c r="AA65" s="54"/>
+      <c r="AB65" s="54"/>
+      <c r="AC65" s="54"/>
+      <c r="AD65" s="54"/>
+      <c r="AE65" s="55"/>
+    </row>
+    <row r="66" spans="4:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="E65" s="67"/>
-      <c r="F65" s="67"/>
-      <c r="G65" s="67"/>
-      <c r="H65" s="67"/>
-      <c r="I65" s="67"/>
-      <c r="J65" s="67"/>
-      <c r="K65" s="67"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="60"/>
-      <c r="O65" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="P65" s="51"/>
-      <c r="Q65" s="51"/>
-      <c r="R65" s="51"/>
-      <c r="S65" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="T65" s="51"/>
-      <c r="U65" s="51"/>
-      <c r="V65" s="51"/>
-      <c r="W65" s="51"/>
-      <c r="X65" s="51"/>
-      <c r="Y65" s="51"/>
-      <c r="Z65" s="51"/>
-      <c r="AA65" s="51"/>
-      <c r="AB65" s="51"/>
-      <c r="AC65" s="51"/>
-      <c r="AD65" s="51"/>
-      <c r="AE65" s="52"/>
-    </row>
-    <row r="66" spans="4:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="48" t="s">
+      <c r="E66" s="52"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="64"/>
+      <c r="M66" s="65"/>
+      <c r="O66" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="P66" s="50"/>
+      <c r="Q66" s="50"/>
+      <c r="R66" s="50"/>
+      <c r="S66" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="T66" s="50"/>
+      <c r="U66" s="50"/>
+      <c r="V66" s="50"/>
+      <c r="W66" s="50"/>
+      <c r="X66" s="50"/>
+      <c r="Y66" s="50"/>
+      <c r="Z66" s="50"/>
+      <c r="AA66" s="50"/>
+      <c r="AB66" s="50"/>
+      <c r="AC66" s="50"/>
+      <c r="AD66" s="50"/>
+      <c r="AE66" s="57"/>
+    </row>
+    <row r="67" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="50"/>
+      <c r="K67" s="50"/>
+      <c r="L67" s="59"/>
+      <c r="M67" s="59"/>
+      <c r="O67" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="P67" s="50"/>
+      <c r="Q67" s="50"/>
+      <c r="R67" s="50"/>
+      <c r="S67" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="T67" s="50"/>
+      <c r="U67" s="50"/>
+      <c r="V67" s="50"/>
+      <c r="W67" s="50"/>
+      <c r="X67" s="50"/>
+      <c r="Y67" s="50"/>
+      <c r="Z67" s="50"/>
+      <c r="AA67" s="50"/>
+      <c r="AB67" s="50"/>
+      <c r="AC67" s="50"/>
+      <c r="AD67" s="50"/>
+      <c r="AE67" s="57"/>
+    </row>
+    <row r="68" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="50"/>
+      <c r="H68" s="50"/>
+      <c r="I68" s="50"/>
+      <c r="J68" s="50"/>
+      <c r="K68" s="50"/>
+      <c r="L68" s="59"/>
+      <c r="M68" s="59"/>
+      <c r="O68" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="P68" s="50"/>
+      <c r="Q68" s="50"/>
+      <c r="R68" s="50"/>
+      <c r="S68" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T68" s="50"/>
+      <c r="U68" s="50"/>
+      <c r="V68" s="50"/>
+      <c r="W68" s="50"/>
+      <c r="X68" s="50"/>
+      <c r="Y68" s="50"/>
+      <c r="Z68" s="50"/>
+      <c r="AA68" s="50"/>
+      <c r="AB68" s="50"/>
+      <c r="AC68" s="50"/>
+      <c r="AD68" s="50"/>
+      <c r="AE68" s="57"/>
+    </row>
+    <row r="69" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="50"/>
+      <c r="I69" s="50"/>
+      <c r="J69" s="50"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="59"/>
+      <c r="M69" s="59"/>
+      <c r="O69" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="P69" s="50"/>
+      <c r="Q69" s="50"/>
+      <c r="R69" s="50"/>
+      <c r="S69" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
-      <c r="I66" s="49"/>
-      <c r="J66" s="49"/>
-      <c r="K66" s="49"/>
-      <c r="L66" s="61"/>
-      <c r="M66" s="62"/>
-      <c r="O66" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="P66" s="47"/>
-      <c r="Q66" s="47"/>
-      <c r="R66" s="47"/>
-      <c r="S66" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="T66" s="47"/>
-      <c r="U66" s="47"/>
-      <c r="V66" s="47"/>
-      <c r="W66" s="47"/>
-      <c r="X66" s="47"/>
-      <c r="Y66" s="47"/>
-      <c r="Z66" s="47"/>
-      <c r="AA66" s="47"/>
-      <c r="AB66" s="47"/>
-      <c r="AC66" s="47"/>
-      <c r="AD66" s="47"/>
-      <c r="AE66" s="54"/>
-    </row>
-    <row r="67" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="56"/>
-      <c r="M67" s="56"/>
-      <c r="O67" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="P67" s="47"/>
-      <c r="Q67" s="47"/>
-      <c r="R67" s="47"/>
-      <c r="S67" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="T67" s="47"/>
-      <c r="U67" s="47"/>
-      <c r="V67" s="47"/>
-      <c r="W67" s="47"/>
-      <c r="X67" s="47"/>
-      <c r="Y67" s="47"/>
-      <c r="Z67" s="47"/>
-      <c r="AA67" s="47"/>
-      <c r="AB67" s="47"/>
-      <c r="AC67" s="47"/>
-      <c r="AD67" s="47"/>
-      <c r="AE67" s="54"/>
-    </row>
-    <row r="68" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-      <c r="K68" s="47"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="56"/>
-      <c r="O68" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="P68" s="47"/>
-      <c r="Q68" s="47"/>
-      <c r="R68" s="47"/>
-      <c r="S68" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="T68" s="47"/>
-      <c r="U68" s="47"/>
-      <c r="V68" s="47"/>
-      <c r="W68" s="47"/>
-      <c r="X68" s="47"/>
-      <c r="Y68" s="47"/>
-      <c r="Z68" s="47"/>
-      <c r="AA68" s="47"/>
-      <c r="AB68" s="47"/>
-      <c r="AC68" s="47"/>
-      <c r="AD68" s="47"/>
-      <c r="AE68" s="54"/>
-    </row>
-    <row r="69" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="47"/>
-      <c r="L69" s="56"/>
-      <c r="M69" s="56"/>
-      <c r="O69" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="P69" s="47"/>
-      <c r="Q69" s="47"/>
-      <c r="R69" s="47"/>
-      <c r="S69" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="T69" s="47"/>
-      <c r="U69" s="47"/>
-      <c r="V69" s="47"/>
-      <c r="W69" s="47"/>
-      <c r="X69" s="47"/>
-      <c r="Y69" s="47"/>
-      <c r="Z69" s="47"/>
-      <c r="AA69" s="47"/>
-      <c r="AB69" s="47"/>
-      <c r="AC69" s="47"/>
-      <c r="AD69" s="47"/>
-      <c r="AE69" s="54"/>
+      <c r="T69" s="50"/>
+      <c r="U69" s="50"/>
+      <c r="V69" s="50"/>
+      <c r="W69" s="50"/>
+      <c r="X69" s="50"/>
+      <c r="Y69" s="50"/>
+      <c r="Z69" s="50"/>
+      <c r="AA69" s="50"/>
+      <c r="AB69" s="50"/>
+      <c r="AC69" s="50"/>
+      <c r="AD69" s="50"/>
+      <c r="AE69" s="57"/>
     </row>
     <row r="70" spans="4:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="47"/>
-      <c r="L70" s="56"/>
-      <c r="M70" s="56"/>
-      <c r="O70" s="48" t="s">
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="59"/>
+      <c r="M70" s="59"/>
+      <c r="O70" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="P70" s="49"/>
-      <c r="Q70" s="49"/>
-      <c r="R70" s="49"/>
-      <c r="S70" s="49" t="s">
+      <c r="P70" s="52"/>
+      <c r="Q70" s="52"/>
+      <c r="R70" s="52"/>
+      <c r="S70" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="T70" s="49"/>
-      <c r="U70" s="49"/>
-      <c r="V70" s="49"/>
-      <c r="W70" s="49"/>
-      <c r="X70" s="49"/>
-      <c r="Y70" s="49"/>
-      <c r="Z70" s="49"/>
-      <c r="AA70" s="49"/>
-      <c r="AB70" s="49"/>
-      <c r="AC70" s="49"/>
-      <c r="AD70" s="49"/>
-      <c r="AE70" s="55"/>
+      <c r="T70" s="52"/>
+      <c r="U70" s="52"/>
+      <c r="V70" s="52"/>
+      <c r="W70" s="52"/>
+      <c r="X70" s="52"/>
+      <c r="Y70" s="52"/>
+      <c r="Z70" s="52"/>
+      <c r="AA70" s="52"/>
+      <c r="AB70" s="52"/>
+      <c r="AC70" s="52"/>
+      <c r="AD70" s="52"/>
+      <c r="AE70" s="58"/>
     </row>
     <row r="71" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3909,7 +3971,7 @@
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="AG55:AH56"/>
     <mergeCell ref="AD47:AE48"/>
-    <mergeCell ref="AF61:AG62"/>
+    <mergeCell ref="AH61:AI62"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="C29:C30"/>
@@ -3926,6 +3988,11 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="AJ61:AK62"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
@@ -3950,11 +4017,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C23:C24"/>

</xml_diff>